<commit_message>
Created Updated Budget Summary Report (still in draft form)
</commit_message>
<xml_diff>
--- a/data/Budget Data.xlsx
+++ b/data/Budget Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissa/Library/CloudStorage/Dropbox/GitHub/PCCFA_25_28_negotiations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3077B2-91EE-134D-815D-1E5FD43C79F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59A6AE4-0AC5-3342-9BF3-D4819A9C6291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16120" xr2:uid="{0DA70FDD-596E-F446-80F6-CC2759EC22CB}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Total Compensation</t>
-  </si>
-  <si>
     <t>Actual Total Income</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>Budget Total Compensation</t>
+  </si>
+  <si>
+    <t>Actual Total Compensation</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,22 +510,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>

</xml_diff>